<commit_message>
csoportbeosztáshoz Roland része egyenlőre Datascan2 és Timetable2 osztályokat hoztam létre és azokban módosítottam, hogy a régi verzió is működőképes maradjon amíg nincs kész teljesen az új
</commit_message>
<xml_diff>
--- a/src/schedule/data/Egy jó órarend.xlsx
+++ b/src/schedule/data/Egy jó órarend.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felhasznalo\Desktop\képzés\Java képzés\ak_iterator\_000000 Projekt\SchoolSchedule\src\schedule\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FA3503-D4FA-46D1-A563-0BF41815A752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1A41DB-AC21-490C-9D45-A049C5A9BA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1066,7 +1066,7 @@
   <dimension ref="B3:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>